<commit_message>
updated list of questions and fixed code
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/Local Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B12CBC-7F38-514F-A7D8-0657AA11745E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEED72CA-25BF-984E-9F55-0AF13504FF11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14080" yWindow="500" windowWidth="14720" windowHeight="16300" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -149,10 +149,13 @@
     <t>interpret CI &amp; PI from a simple lm model</t>
   </si>
   <si>
-    <t>interpret slope, interpret intercept</t>
-  </si>
-  <si>
     <t>slope estimate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">which plot to assess? &amp; which seems reasonable? : linearity </t>
+  </si>
+  <si>
+    <t>interpret slope, interpret intercept, assumptions of lm check</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -750,7 +753,7 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -769,7 +772,7 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -778,6 +781,9 @@
       </c>
       <c r="B24">
         <v>7</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
breaking up old 2 sample ttest questions
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/Local Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB71E97-32C3-2E4E-8887-24D8E8CC1C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B8064E-CBD5-9041-9F32-BAB31835D9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -165,6 +165,15 @@
   </si>
   <si>
     <t>lm-linearity-check, lm-linearity-plots, lm-normality-check, lm-normality-plots, lm-homoscedasticity-check, lm-homoscedasticity-plots</t>
+  </si>
+  <si>
+    <t>single choice</t>
+  </si>
+  <si>
+    <t>read test-statistic, read sided t-test</t>
+  </si>
+  <si>
+    <t>schoice-2samtt-interpret-t, schoice-2samtt-interpret-alt</t>
   </si>
 </sst>
 </file>
@@ -550,7 +559,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,7 +636,7 @@
         <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -758,9 +767,15 @@
       <c r="B16" s="2">
         <v>5</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">

</xml_diff>

<commit_message>
changed file name, updated excel
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/Local Documents/quizbank/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1825938/Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B8064E-CBD5-9041-9F32-BAB31835D9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EF7CB6-996D-554C-B67C-E61AE41D8AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>num</t>
   </si>
   <si>
-    <t>mult choice</t>
-  </si>
-  <si>
     <t>What is the interquartile range of the following sample:</t>
   </si>
   <si>
@@ -173,7 +170,10 @@
     <t>read test-statistic, read sided t-test</t>
   </si>
   <si>
-    <t>schoice-2samtt-interpret-t, schoice-2samtt-interpret-alt</t>
+    <t>schoice-2samtt-interpret-t, schoice-2samtt-interpret-alt, schoice-2samtt-interpret-p</t>
+  </si>
+  <si>
+    <t>schoice</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>14</v>
@@ -599,7 +599,7 @@
         <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>15</v>
@@ -616,7 +616,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>15</v>
@@ -630,13 +630,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -707,7 +707,7 @@
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="2">
         <v>5</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2">
         <v>5</v>
@@ -729,18 +729,24 @@
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2">
         <v>5</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="2">
         <v>5</v>
@@ -751,7 +757,7 @@
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
         <v>5</v>
@@ -762,24 +768,15 @@
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>5</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2">
         <v>6</v>
@@ -790,7 +787,7 @@
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2">
         <v>6</v>
@@ -801,7 +798,7 @@
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="2">
         <v>6</v>
@@ -812,7 +809,7 @@
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="2">
         <v>6</v>
@@ -823,24 +820,24 @@
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="2">
         <v>7</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="2">
         <v>7</v>
@@ -851,16 +848,16 @@
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="2">
         <v>7</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>15</v>
@@ -868,24 +865,24 @@
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2">
         <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" s="2">
         <v>7</v>

</xml_diff>

<commit_message>
which ttest to use
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1825938/Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EF7CB6-996D-554C-B67C-E61AE41D8AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD67BAAB-3CF4-CB4D-9932-C835362D2B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -174,6 +174,21 @@
   </si>
   <si>
     <t>schoice</t>
+  </si>
+  <si>
+    <t>know which scenario to use t-test</t>
+  </si>
+  <si>
+    <t>which-ttest-to-use</t>
+  </si>
+  <si>
+    <t>Reasonable QQ plots</t>
+  </si>
+  <si>
+    <t>which qqplots seem normally distributed</t>
+  </si>
+  <si>
+    <t>lm-normality-plots</t>
   </si>
 </sst>
 </file>
@@ -556,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770463FC-439A-7843-85D6-C7A4E4EBD8B0}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -707,79 +722,70 @@
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B11" s="2">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="2">
-        <v>5</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="2">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="2">
-        <v>5</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="2">
-        <v>5</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2">
         <v>5</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -787,32 +793,35 @@
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B18" s="2">
-        <v>6</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>6</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -820,27 +829,21 @@
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B21" s="2">
-        <v>7</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -848,33 +851,27 @@
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23" s="2">
-        <v>7</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>45</v>
@@ -882,42 +879,103 @@
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="2">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="2">
+        <v>7</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" s="2">
+        <v>7</v>
+      </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+    <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="2">
+        <v>7</v>
+      </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="2">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
which plots to use question
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1825938/Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD67BAAB-3CF4-CB4D-9932-C835362D2B79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C88183-ED17-B349-AD83-0CCCDA904E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21180" windowHeight="23200" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -164,9 +164,6 @@
     <t>lm-linearity-check, lm-linearity-plots, lm-normality-check, lm-normality-plots, lm-homoscedasticity-check, lm-homoscedasticity-plots</t>
   </si>
   <si>
-    <t>single choice</t>
-  </si>
-  <si>
     <t>read test-statistic, read sided t-test</t>
   </si>
   <si>
@@ -189,6 +186,24 @@
   </si>
   <si>
     <t>lm-normality-plots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding which plot to use </t>
+  </si>
+  <si>
+    <t>penguins-which-plot-to-use</t>
+  </si>
+  <si>
+    <t>Definition of statistic</t>
+  </si>
+  <si>
+    <t>what-does-statistic-mean</t>
+  </si>
+  <si>
+    <t>Calculate statistics in R</t>
+  </si>
+  <si>
+    <t>calculate-stuff-in-R-diamonds</t>
   </si>
 </sst>
 </file>
@@ -573,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770463FC-439A-7843-85D6-C7A4E4EBD8B0}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,7 +666,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -722,39 +737,59 @@
     </row>
     <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2">
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
@@ -771,13 +806,13 @@
         <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -799,13 +834,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -874,7 +909,7 @@
         <v>38</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -919,7 +954,7 @@
         <v>41</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update list of questions
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1825938/Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C88183-ED17-B349-AD83-0CCCDA904E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2015BD0-8A86-DF41-96ED-AF769B460611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="21180" windowHeight="23200" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -204,6 +204,21 @@
   </si>
   <si>
     <t>calculate-stuff-in-R-diamonds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Understanding quantitative, continuous, categorical, ordinal etc </t>
+  </si>
+  <si>
+    <t>what-type-of-variable</t>
+  </si>
+  <si>
+    <t>Understanding subjects and variables of a setting</t>
+  </si>
+  <si>
+    <t>what-are-the-subjects-and-variables</t>
+  </si>
+  <si>
+    <t>w</t>
   </si>
 </sst>
 </file>
@@ -586,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770463FC-439A-7843-85D6-C7A4E4EBD8B0}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,36 +795,38 @@
     </row>
     <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="2">
-        <v>5</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>44</v>
@@ -817,54 +834,60 @@
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
         <v>5</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" s="2">
         <v>5</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2">
         <v>5</v>
       </c>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2">
         <v>5</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2">
         <v>5</v>
@@ -875,10 +898,10 @@
     </row>
     <row r="22" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -886,7 +909,7 @@
     </row>
     <row r="23" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2">
         <v>6</v>
@@ -897,80 +920,80 @@
     </row>
     <row r="24" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" s="2">
         <v>6</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>44</v>
-      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="2">
         <v>6</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+    </row>
+    <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B26" s="2">
-        <v>7</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="B27" s="2">
         <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>7</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2">
         <v>7</v>
@@ -981,7 +1004,7 @@
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2">
         <v>7</v>
@@ -990,9 +1013,13 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+    <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>7</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1004,13 +1031,20 @@
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more new questions !
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/Local Documents/quizbank/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1825938/Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC1D532-1107-2E43-B70F-FA72E0D800D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBB2196-AEF2-CA49-816A-EAD3F3E8FA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16320" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
+    <workbookView xWindow="24440" yWindow="500" windowWidth="20360" windowHeight="23180" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="71">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>matched-pairs-t-test-assumptions, matched-pairs-t-test-assumptions-2</t>
+  </si>
+  <si>
+    <t>matched-pairs-ttest-CI</t>
   </si>
 </sst>
 </file>
@@ -634,7 +637,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="93" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,7 +975,9 @@
         <v>5</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
week 1 questions complete
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a1825938/Documents/quizbank/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/Local Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B8EF75-CDA5-D644-825C-8CF883905C06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A00D357-C3BA-C547-8CAB-B8CD605855E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24600" yWindow="500" windowWidth="20200" windowHeight="23200" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -209,9 +209,6 @@
     <t>calculate-stuff-in-R-diamonds, schoice-calculate-IQR, calculate-sample-mean, calculate-median</t>
   </si>
   <si>
-    <t>what-type-of-variable,</t>
-  </si>
-  <si>
     <t>schoice-2samtt-interpret-t</t>
   </si>
   <si>
@@ -224,13 +221,28 @@
     <t>interpret slope, interpret intercept, assumptions of lm check, linear-model-slope</t>
   </si>
   <si>
-    <t xml:space="preserve"> what-are-the-subjects-and-variables, identify-response-and-explanatory-vars</t>
-  </si>
-  <si>
     <t>what-does-statistic-mean, affected-by-skewness</t>
   </si>
   <si>
-    <t>anova-fraction-of-var-explained, anova-sided-test, anova-test-stat</t>
+    <t>interpretation-coffee</t>
+  </si>
+  <si>
+    <t>sampling-bias-which-type, scientific-reasoning-coin, reliability-vs-validity</t>
+  </si>
+  <si>
+    <t>what-type-of-variable, identify-sample-space-and-variable-type-coin, identify-sample-space-and-variable-type-dice</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> what-are-the-subjects-and-variables, identify-response-and-explanatory-vars, rectangular-data-interpretation, identify-subjects-and-variables</t>
+  </si>
+  <si>
+    <t>anova-fraction-of-var-explained, anova-sided-test, anova-test-stat, anova-assumptions</t>
+  </si>
+  <si>
+    <t>anova-two-way-which-code-interaction, anova-two-way-interaction-means, anova-one-way-purpose, anova-one-way-sided-test,</t>
+  </si>
+  <si>
+    <t>anova-two-way-conclusion, anova-two-way-significant-terms,  anova-one-way-interpret</t>
   </si>
 </sst>
 </file>
@@ -627,17 +639,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770463FC-439A-7843-85D6-C7A4E4EBD8B0}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="93" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="108" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="94.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -666,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
@@ -680,7 +692,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>57</v>
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
@@ -690,6 +705,9 @@
       <c r="B4" s="2">
         <v>1</v>
       </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -699,15 +717,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -729,7 +753,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>8</v>
@@ -752,7 +776,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
@@ -769,7 +793,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>31</v>
       </c>
@@ -786,7 +810,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
@@ -802,7 +826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>16</v>
       </c>
@@ -844,7 +868,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>34</v>
       </c>
@@ -855,13 +879,13 @@
         <v>9</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>35</v>
       </c>
@@ -869,10 +893,10 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -880,7 +904,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>8</v>
@@ -894,7 +918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
@@ -910,7 +934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>40</v>
       </c>
@@ -918,7 +942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>41</v>
       </c>
@@ -926,7 +950,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>42</v>
       </c>
@@ -943,7 +967,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>43</v>
       </c>
@@ -951,7 +975,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>5</v>
@@ -960,7 +984,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>44</v>
       </c>
@@ -968,7 +992,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -1023,6 +1047,12 @@
       <c r="B34" s="2">
         <v>9</v>
       </c>
+      <c r="D34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
@@ -1032,7 +1062,7 @@
         <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1044,6 +1074,12 @@
       </c>
       <c r="B36" s="2">
         <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
mann whitney and chisq
</commit_message>
<xml_diff>
--- a/list-of-questions.xlsx
+++ b/list-of-questions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jj/Local Documents/quizbank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF760698-8716-714A-B1AB-29A4939DEF61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1583EB-6400-9A43-A9BB-BCD945C1FB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-160" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
+    <workbookView xWindow="-100" yWindow="500" windowWidth="28800" windowHeight="16340" xr2:uid="{F5571BD5-EB0B-EE4E-9552-527778988CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="76">
   <si>
     <t xml:space="preserve">Question </t>
   </si>
@@ -252,6 +252,18 @@
   </si>
   <si>
     <t>two-sample-t-test-interpret-t, two-sample-t-test-interpret-alt, two-sample-t-test-interpret-p, matched-pairs-t-test-CI, matched-pairs-t-test-conclusion, matched-pairs-t-test-ci-interpret, matched-pairs-t-test-what -parameters-tested, matched-pairs-t-test-null-and-alt-hyp,matched-pairs-t-test-retain-or-reject, one-sample-t-test-what does-test-stat-mean, one-sample-t-test-rejct-or-retain-using-CI, one-sample-t-test-95-ci-interpret, one-sample-t-test-conclusion, one-sample-t-test-null-and-alt</t>
+  </si>
+  <si>
+    <t>chi-square-interpret-output</t>
+  </si>
+  <si>
+    <t>chi-square-when-to-use, chi-square-null-hyp, chi-square-which-code</t>
+  </si>
+  <si>
+    <t>mann-whitney-interpret-results</t>
+  </si>
+  <si>
+    <t>mann-whitney-which-code, mann-whitney-null-and-alt-hyp, mann-whitney-when-to-use</t>
   </si>
 </sst>
 </file>
@@ -650,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770463FC-439A-7843-85D6-C7A4E4EBD8B0}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D19" activeCellId="1" sqref="D25 D19"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="94" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -959,7 +971,9 @@
         <v>6</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -970,7 +984,9 @@
         <v>6</v>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -981,7 +997,9 @@
         <v>6</v>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="E22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -992,7 +1010,9 @@
         <v>6</v>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="D23" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1003,7 +1023,6 @@
         <v>7</v>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">

</xml_diff>